<commit_message>
Improving tests and coverage
</commit_message>
<xml_diff>
--- a/tests/data/licenses_v2.xlsx
+++ b/tests/data/licenses_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="182">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -563,6 +563,9 @@
   </si>
   <si>
     <t xml:space="preserve">This work is protected under the Copyright Act No. 121/2000 Coll.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test slugify</t>
   </si>
 </sst>
 </file>
@@ -805,7 +808,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2022,6 +2025,17 @@
         <v>180</v>
       </c>
     </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added recognition list feature
</commit_message>
<xml_diff>
--- a/tests/data/licenses_v2.xlsx
+++ b/tests/data/licenses_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="186">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">title_sk</t>
   </si>
   <si>
+    <t xml:space="preserve">list</t>
+  </si>
+  <si>
     <t xml:space="preserve">CC</t>
   </si>
   <si>
@@ -569,6 +572,9 @@
   </si>
   <si>
     <t xml:space="preserve">test other language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['C01', 'C01.252', 'C01.252.400']</t>
   </si>
   <si>
     <t xml:space="preserve">test slugify</t>
@@ -582,7 +588,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -630,6 +636,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -684,7 +696,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -730,6 +742,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -807,14 +823,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -914,7 +930,9 @@
       <c r="G5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="0"/>
+      <c r="H5" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -937,13 +955,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -967,13 +985,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -997,19 +1015,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -1031,19 +1049,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1065,19 +1083,19 @@
         <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -1099,19 +1117,19 @@
         <v>3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -1133,19 +1151,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -1167,19 +1185,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1201,13 +1219,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1231,19 +1249,19 @@
         <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1265,19 +1283,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -1299,19 +1317,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1333,19 +1351,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -1367,19 +1385,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -1401,19 +1419,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -1435,13 +1453,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1465,19 +1483,19 @@
         <v>3</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -1499,19 +1517,19 @@
         <v>3</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -1533,19 +1551,19 @@
         <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -1567,19 +1585,19 @@
         <v>3</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
@@ -1601,19 +1619,19 @@
         <v>3</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
@@ -1635,19 +1653,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -1669,13 +1687,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -1699,19 +1717,19 @@
         <v>3</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -1733,19 +1751,19 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -1767,19 +1785,19 @@
         <v>3</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -1801,19 +1819,19 @@
         <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
@@ -1835,19 +1853,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
@@ -1869,19 +1887,19 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,13 +1907,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E35" s="6"/>
     </row>
@@ -1904,19 +1922,19 @@
         <v>3</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,19 +1942,19 @@
         <v>3</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,19 +1962,19 @@
         <v>3</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,19 +1982,19 @@
         <v>3</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,19 +2002,19 @@
         <v>3</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,19 +2022,19 @@
         <v>3</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,16 +2042,19 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2041,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>